<commit_message>
Experimental Velocity Data 6L 2500RPM
</commit_message>
<xml_diff>
--- a/Velocity_Data/Experimental_6L_2500/Q2_6L_2500.xlsx
+++ b/Velocity_Data/Experimental_6L_2500/Q2_6L_2500.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joseph Tarriela\Documents\GitHub\FDA_Blood_Pump\Velocity_Data\Experimental_6L_2500\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{64EB2194-CAF3-4EBB-8853-5B26ABA91E76}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1FB27B-57E6-4B3C-A0F3-80EEF63F8127}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10770" yWindow="4810" windowWidth="33340" windowHeight="20440" xr2:uid="{D44E2806-618A-4F4E-9228-DC91233EC85A}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="33340" windowHeight="20440" xr2:uid="{D44E2806-618A-4F4E-9228-DC91233EC85A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Q1 Velocity Magnitude</t>
-  </si>
-  <si>
     <t>nodenumber</t>
   </si>
   <si>
@@ -49,6 +46,9 @@
   </si>
   <si>
     <t xml:space="preserve">    z-coordinate</t>
+  </si>
+  <si>
+    <t>Q2 Velocity Magnitude</t>
   </si>
 </sst>
 </file>
@@ -477,26 +477,26 @@
   <dimension ref="A1:E48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>4</v>
-      </c>
-      <c r="E1" t="s">
-        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>